<commit_message>
UV and Model updates
Updates to models with uvs and those models added to unity for testing, also other quality of life improvements to the level
</commit_message>
<xml_diff>
--- a/SleuthPlans.xlsx
+++ b/SleuthPlans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210421\Documents\bankruptcy\Project_Sleuth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721254E2-3A86-41AB-AA52-9CCD9043EADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240F999B-5ED4-4B97-96EC-8C4716BFEDA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{1D43F9DA-CECD-4A9A-9825-4B9F9954E114}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D43F9DA-CECD-4A9A-9825-4B9F9954E114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,12 +188,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -243,6 +237,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8C00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,23 +265,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,16 +359,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FFFFA500"/>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF8C00"/>
-      <color rgb="FFFFA500"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FFDDDDDD"/>
       <color rgb="FF969696"/>
       <color rgb="FF333333"/>
       <color rgb="FF000000"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FF1C1C1C"/>
-      <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -689,7 +699,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,297 +724,301 @@
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>6</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>5</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="12"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>5</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="12"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="H6" s="6"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="H7" s="6"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="H8" s="6"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>4</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>4</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>4</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="H11" s="6"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>3</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>3</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>3</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>3</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>3</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>2</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>2</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>2</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>2</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>2</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="8">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>1</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>1</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>1</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="8">
         <v>1</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">

</xml_diff>

<commit_message>
Models Uv And Level Update
New Models,
New textures
and changes to the level have been made
</commit_message>
<xml_diff>
--- a/SleuthPlans.xlsx
+++ b/SleuthPlans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210421\Documents\bankruptcy\Project_Sleuth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FCD515-C71A-408E-BCAB-952361998DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC7C7A-A652-4E50-A148-8BF7B07C1735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D43F9DA-CECD-4A9A-9825-4B9F9954E114}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Asset</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Pillar/</t>
-  </si>
-  <si>
-    <t>Desk/</t>
   </si>
   <si>
     <t>Bed/</t>
@@ -293,8 +290,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,10 +365,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFFA500"/>
       <color rgb="FFFF8C00"/>
-      <color rgb="FF00FF00"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFDDDDDD"/>
       <color rgb="FF969696"/>
       <color rgb="FF333333"/>
@@ -708,7 +705,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +743,7 @@
         <v>17</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,8 +753,9 @@
       <c r="B2" s="4">
         <v>6</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="19"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -809,8 +807,8 @@
       <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -826,7 +824,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="6">
         <v>4</v>
@@ -837,17 +835,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6">
         <v>4</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6">
         <v>4</v>
@@ -873,17 +873,20 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="7">
         <v>3</v>
@@ -893,7 +896,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
@@ -903,7 +906,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
@@ -913,7 +916,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7">
         <v>3</v>
@@ -923,12 +926,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="7">
         <v>3</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1033,7 +1040,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>